<commit_message>
Test Suite Execution Engine
</commit_message>
<xml_diff>
--- a/src/test/resources/dataEngine/DataEngine.xlsx
+++ b/src/test/resources/dataEngine/DataEngine.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium Projects\KeyworddrivenFramework\src\test\resources\dataEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75EA79F6-A8D5-435B-8D35-15E163F63EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CE7E8B-BFA4-488D-9BA3-890C6554F376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="830" yWindow="2160" windowWidth="18370" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Steps" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Cases" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -94,6 +95,45 @@
   </si>
   <si>
     <t>doClose</t>
+  </si>
+  <si>
+    <t>Page Objects</t>
+  </si>
+  <si>
+    <t>txtbx_UserName</t>
+  </si>
+  <si>
+    <t>txtbx_Password</t>
+  </si>
+  <si>
+    <t>btn_LogIn</t>
+  </si>
+  <si>
+    <t>TS_007</t>
+  </si>
+  <si>
+    <t>Click LogOut Button</t>
+  </si>
+  <si>
+    <t>btn_Signout</t>
+  </si>
+  <si>
+    <t>doLogout</t>
+  </si>
+  <si>
+    <t>Runmode</t>
+  </si>
+  <si>
+    <t>Login_02</t>
+  </si>
+  <si>
+    <t>Login to the online app</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -417,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -428,9 +468,10 @@
     <col min="1" max="1" width="12.26953125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="17.26953125" customWidth="1"/>
+    <col min="5" max="5" width="16.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,10 +482,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -454,11 +498,11 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -468,11 +512,11 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -483,10 +527,13 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -497,10 +544,13 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -511,10 +561,13 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -522,10 +575,80 @@
         <v>16</v>
       </c>
       <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
         <v>13</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E8" t="s">
         <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D50F85A5-737C-4BE3-BEDF-19B7A527B647}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.26953125" customWidth="1"/>
+    <col min="2" max="2" width="22.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>